<commit_message>
excel practical, vloopup, hloopup
</commit_message>
<xml_diff>
--- a/MCQ/practical/mark-parcentage.xlsx
+++ b/MCQ/practical/mark-parcentage.xlsx
@@ -137,7 +137,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -165,6 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -460,7 +461,7 @@
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C1">
         <f ca="1">RANDBETWEEN(1,60)</f>
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E1" t="str">
         <f>CHOOSE(3,"John","Alice","Bob","Emma")</f>
@@ -666,11 +667,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E3:K20"/>
+  <dimension ref="E1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5:I9"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,6 +685,16 @@
     <col min="11" max="11" width="31" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H1" t="str">
+        <f>(35/50)*100 &amp; "%"</f>
+        <v>70%</v>
+      </c>
+      <c r="I1" s="11">
+        <f>(44/50)*100</f>
+        <v>88</v>
+      </c>
+    </row>
     <row r="3" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -927,5 +938,6 @@
     <mergeCell ref="E18:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>